<commit_message>
Analysis of proiel stats.
</commit_message>
<xml_diff>
--- a/R_files/Rresults/statsRelPos/Polybius_comparison/PolybiusAnalysis.xlsx
+++ b/R_files/Rresults/statsRelPos/Polybius_comparison/PolybiusAnalysis.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="150" windowWidth="18180" windowHeight="6770" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="210" windowWidth="18180" windowHeight="6710" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="zscores_Oct11" sheetId="1" r:id="rId1"/>
     <sheet name="working" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2223" uniqueCount="565">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2249" uniqueCount="565">
   <si>
     <t>Aeschylus</t>
   </si>
@@ -2541,13 +2542,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AOS21"/>
+  <dimension ref="A1:AOU21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="J4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="P1" sqref="P1:Q18"/>
+      <selection pane="bottomRight" sqref="A1:A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3114,7 +3115,7 @@
     <col min="1084" max="1085" width="22.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1085" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1087" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>557</v>
       </c>
@@ -6371,7 +6372,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="2" spans="1:1085" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1087" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>558</v>
       </c>
@@ -9628,7 +9629,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="3" spans="1:1085" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1087" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>559</v>
       </c>
@@ -12885,7 +12886,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="4" spans="1:1085" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1087" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -16142,7 +16143,7 @@
         <v>1.08403094030971E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:1085" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1087" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -19399,7 +19400,7 @@
         <v>-0.28176448203578902</v>
       </c>
     </row>
-    <row r="6" spans="1:1085" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1087" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -22656,7 +22657,7 @@
         <v>-0.73835128063665401</v>
       </c>
     </row>
-    <row r="7" spans="1:1085" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1087" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -25913,7 +25914,7 @@
         <v>5.14033498625883E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:1085" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:1087" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -29170,7 +29171,7 @@
         <v>3.2466162946014698</v>
       </c>
     </row>
-    <row r="9" spans="1:1085" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:1087" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -32427,7 +32428,7 @@
         <v>0.52989635637380295</v>
       </c>
     </row>
-    <row r="10" spans="1:1085" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:1087" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -35684,7 +35685,7 @@
         <v>0.74088976397383</v>
       </c>
     </row>
-    <row r="11" spans="1:1085" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:1087" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -38940,8 +38941,12 @@
       <c r="AOS11">
         <v>-0.57924502394509703</v>
       </c>
+      <c r="AOU11">
+        <f>LARGE(B4:AOS18, 2)</f>
+        <v>3.61478445646026</v>
+      </c>
     </row>
-    <row r="12" spans="1:1085" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:1087" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -42198,7 +42203,7 @@
         <v>-0.73835128063665401</v>
       </c>
     </row>
-    <row r="13" spans="1:1085" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:1087" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -45455,7 +45460,7 @@
         <v>-0.237334782920188</v>
       </c>
     </row>
-    <row r="14" spans="1:1085" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:1087" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -48712,7 +48717,7 @@
         <v>-2.2887776747468301E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:1085" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:1087" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>11</v>
       </c>
@@ -51969,7 +51974,7 @@
         <v>-0.73835128063665401</v>
       </c>
     </row>
-    <row r="16" spans="1:1085" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:1087" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>12</v>
       </c>
@@ -62024,7 +62029,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
@@ -62720,7 +62725,7 @@
         <v>1.1503742462599918E-2</v>
       </c>
       <c r="N20">
-        <f t="shared" ref="L20:N20" si="6">AVERAGE(N4:N18)</f>
+        <f t="shared" ref="N20" si="6">AVERAGE(N4:N18)</f>
         <v>0.30480685165303728</v>
       </c>
     </row>
@@ -62745,7 +62750,7 @@
         <v>4.4945705695754665E-3</v>
       </c>
       <c r="N21">
-        <f t="shared" ref="L21:N21" si="9">_xlfn.STDEV.S(N4:N18)</f>
+        <f t="shared" ref="N21" si="9">_xlfn.STDEV.S(N4:N18)</f>
         <v>9.8689043383668767E-2</v>
       </c>
     </row>
@@ -62753,4 +62758,468 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="M4" sqref="M4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>557</v>
+      </c>
+      <c r="B1">
+        <v>2</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="I1">
+        <v>32</v>
+      </c>
+      <c r="J1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>558</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>559</v>
+      </c>
+      <c r="B3" t="s">
+        <v>560</v>
+      </c>
+      <c r="C3" t="s">
+        <v>561</v>
+      </c>
+      <c r="I3" t="s">
+        <v>560</v>
+      </c>
+      <c r="J3" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>5.8922221665748502E-2</v>
+      </c>
+      <c r="C4">
+        <v>1.82954911130881</v>
+      </c>
+      <c r="I4">
+        <v>2.0283467721740902E-3</v>
+      </c>
+      <c r="J4">
+        <v>-0.74318299398398002</v>
+      </c>
+      <c r="L4">
+        <f>I4/B4</f>
+        <v>3.4424139396515126E-2</v>
+      </c>
+      <c r="M4">
+        <f>STANDARDIZE(L4,$L$20,$L$21)</f>
+        <v>-0.92929966969840672</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>4.3349182419111697E-2</v>
+      </c>
+      <c r="C5">
+        <v>0.43445836703463803</v>
+      </c>
+      <c r="I5">
+        <v>4.1980749159225301E-3</v>
+      </c>
+      <c r="J5">
+        <v>0.82689630909480305</v>
+      </c>
+      <c r="L5">
+        <f t="shared" ref="L5:L18" si="0">I5/B5</f>
+        <v>9.6843231674692248E-2</v>
+      </c>
+      <c r="M5">
+        <f t="shared" ref="M5:M18" si="1">STANDARDIZE(L5,$L$20,$L$21)</f>
+        <v>0.10109630951702138</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>2.5141394542377099E-2</v>
+      </c>
+      <c r="C6">
+        <v>-1.1966629534889499</v>
+      </c>
+      <c r="I6">
+        <v>4.4172893530941698E-3</v>
+      </c>
+      <c r="J6">
+        <v>0.985526343797966</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="0"/>
+        <v>0.17569786535303775</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="1"/>
+        <v>1.4028053622947678</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>3.30252262661275E-2</v>
+      </c>
+      <c r="C7">
+        <v>-0.49040000166376202</v>
+      </c>
+      <c r="I7">
+        <v>3.3699210475640301E-3</v>
+      </c>
+      <c r="J7">
+        <v>0.22761973510523301</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="0"/>
+        <v>0.1020408163265306</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="1"/>
+        <v>0.18689650512093064</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>4.8313090418353598E-2</v>
+      </c>
+      <c r="C8">
+        <v>0.87914369759183697</v>
+      </c>
+      <c r="I8">
+        <v>2.1592442645074201E-3</v>
+      </c>
+      <c r="J8">
+        <v>-0.64846170637491296</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="0"/>
+        <v>4.469273743016753E-2</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="1"/>
+        <v>-0.75978867971315023</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9">
+        <v>3.9943306274964598E-2</v>
+      </c>
+      <c r="C9">
+        <v>0.129347321618761</v>
+      </c>
+      <c r="I9">
+        <v>3.8654812524159302E-3</v>
+      </c>
+      <c r="J9">
+        <v>0.58622172093892599</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="0"/>
+        <v>9.6774193548387136E-2</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="1"/>
+        <v>9.9956648474846546E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10">
+        <v>4.4785091674180898E-2</v>
+      </c>
+      <c r="C10">
+        <v>0.56309245570794497</v>
+      </c>
+      <c r="I10">
+        <v>3.0057108506161699E-3</v>
+      </c>
+      <c r="J10">
+        <v>-3.5933509500869799E-2</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="0"/>
+        <v>6.7114093959731599E-2</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="1"/>
+        <v>-0.38966353413016003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11">
+        <v>4.2052260218060702E-2</v>
+      </c>
+      <c r="C11">
+        <v>0.31827525530706602</v>
+      </c>
+      <c r="I11">
+        <v>2.0933183541183399E-3</v>
+      </c>
+      <c r="J11">
+        <v>-0.69616764028960998</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="0"/>
+        <v>4.9778973669037101E-2</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="1"/>
+        <v>-0.67582659089400055</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12">
+        <v>3.4546680148297898E-2</v>
+      </c>
+      <c r="C12">
+        <v>-0.35410250730572101</v>
+      </c>
+      <c r="I12">
+        <v>2.2750252780586499E-3</v>
+      </c>
+      <c r="J12">
+        <v>-0.56467914882730996</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="0"/>
+        <v>6.5853658536585591E-2</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="1"/>
+        <v>-0.4104704306207777</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13">
+        <v>4.35105722342689E-2</v>
+      </c>
+      <c r="C13">
+        <v>0.44891626659939998</v>
+      </c>
+      <c r="I13">
+        <v>1.8222724450009701E-3</v>
+      </c>
+      <c r="J13">
+        <v>-0.89230445739064801</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="0"/>
+        <v>4.1881141787552714E-2</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="1"/>
+        <v>-0.80620167194986669</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14">
+        <v>2.83969761581702E-2</v>
+      </c>
+      <c r="C14">
+        <v>-0.90501585060227896</v>
+      </c>
+      <c r="I14">
+        <v>2.7137042062415199E-3</v>
+      </c>
+      <c r="J14">
+        <v>-0.24723813308475501</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="0"/>
+        <v>9.5563139931740579E-2</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="1"/>
+        <v>7.9964932292149168E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="2">
+        <v>2.6511489551572801E-2</v>
+      </c>
+      <c r="C15" s="2">
+        <v>-1.0739247496076501</v>
+      </c>
+      <c r="I15" s="2">
+        <v>6.6185766341934999E-3</v>
+      </c>
+      <c r="J15" s="2">
+        <v>2.5784427698225101</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="0"/>
+        <v>0.2496493688639555</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="1"/>
+        <v>2.6235749873158287</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="2">
+        <v>2.6782949736814901E-2</v>
+      </c>
+      <c r="C16" s="2">
+        <v>-1.04960633713386</v>
+      </c>
+      <c r="I16" s="2">
+        <v>4.0251831974403999E-3</v>
+      </c>
+      <c r="J16" s="2">
+        <v>0.70178676039642995</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="0"/>
+        <v>0.15028901734104083</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="1"/>
+        <v>0.98336358779124822</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17">
+        <v>5.7036498224295101E-2</v>
+      </c>
+      <c r="C17">
+        <v>1.6606189957566599</v>
+      </c>
+      <c r="I17">
+        <v>1.7329168627786601E-3</v>
+      </c>
+      <c r="J17">
+        <v>-0.95696479314101801</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="0"/>
+        <v>3.0382595648912259E-2</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="1"/>
+        <v>-0.99601628276279119</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18">
+        <v>2.51745912265295E-2</v>
+      </c>
+      <c r="C18">
+        <v>-1.19368907112289</v>
+      </c>
+      <c r="I18">
+        <v>1.5054572826496001E-3</v>
+      </c>
+      <c r="J18">
+        <v>-1.12156125656276</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="0"/>
+        <v>5.9800664451827065E-2</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="1"/>
+        <v>-0.51039147303764287</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B20">
+        <f t="shared" ref="B20:C20" si="2">AVERAGE(B4:B18)</f>
+        <v>3.8499435383924932E-2</v>
+      </c>
+      <c r="L20">
+        <f>AVERAGE(L4:L18)</f>
+        <v>9.0719042527980923E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B21">
+        <f t="shared" ref="B21:C21" si="3">_xlfn.STDEV.S(B4:B18)</f>
+        <v>1.1162742861389286E-2</v>
+      </c>
+      <c r="L21">
+        <f>_xlfn.STDEV.S(L4:L18)</f>
+        <v>6.057777159195122E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>